<commit_message>
added and updated tests for `getAPAInfo()`
</commit_message>
<xml_diff>
--- a/tests/testthat/helper_getAPAInfo_error3.xlsx
+++ b/tests/testthat/helper_getAPAInfo_error3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\eatPackages\eatCodebook\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50A4757-2E73-459D-9D28-7C98388EBCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CEDD2D-DBDF-4779-8ABB-2973173B8B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quellen Langform" sheetId="2" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FA08BE-260E-4A6A-9BBF-14AB1B2C2E98}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80943FAC-45F0-4F31-9E2E-084AD7C9E4A0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,20 +514,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>